<commit_message>
api routes for daily and history report
</commit_message>
<xml_diff>
--- a/FlagReport.xlsx
+++ b/FlagReport.xlsx
@@ -505,27 +505,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>15455</t>
+          <t>15092</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>26-00</t>
+          <t>21-61</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>B1-008376</t>
+          <t>B1-005812</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>L ENG BTL1 SQUIB</t>
+          <t>ACSC 1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>BOTH BRIDGEWIRES OPEN</t>
+          <t>INTERNAL FAULT</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -535,11 +535,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>L ENG SQUIB (WHITE, AND AMBER)</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="I2" s="2" t="n">
-        <v>44165</v>
+        <v>44161</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>44165</v>
@@ -547,15 +547,25 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fleet wide msg. </t>
+          <t>Per SL-21-018 (to be revised as of 9/24/20)
+This is related to pack cycling. Will have to revise SL procedure (by 30 Sept 2020) and the FIM (31 Oct 2020). (Input from specialist Sep/2020)
+Fleet wide msg in top #10 position
+Reset SL procedure is not in FIM</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Follow FIM TASK 26−21−10−810−801:
-1. Defective bottle 1 L cartridge A256
-2. Defective FIDEEX control unit A136
-3. Defective wiring interface</t>
+          <t>1. Reset per SL procedure: 
+a) Reset procedure
+b) Wait for 30 sec., then select L Pack Manual Mode 
+c) Wait for 30 sec., and then select Pack Auto Mode. 
+d) If still cycling Swap ACSC. If not replace ACSC. Do not remove sensors
+2. Follow FIM 21−61−04−810−81:
+NOTE:Bombardier strongly recommends to swap ASCSs before replacing the LRUs. Byswapping LRUs, you will verify the integrity of the ASCSs. Go to Fault Confirmation.
+1. Pack Discharge Pressure Sensor (PDPS) MT13 unserviceable.
+2. Pack Inlet Flow Sensor (PIFS) MT11 unserviceable.
+3. Pack Inlet Pressure Sensor (PIPS) MT9 unserviceable.
+4. Defective wiring interface between Air Conditioning System Controller #1 (ACSC 1)and oneof the pressure sensors.</t>
         </is>
       </c>
     </row>

</xml_diff>